<commit_message>
Edit & Run Data Prep
Add data files, edit data loading and data prep scripts.
</commit_message>
<xml_diff>
--- a/data/northSeasonalFilter.xlsx
+++ b/data/northSeasonalFilter.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10709"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10414"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/helenkilleen/Desktop/CODING/seabirds-stratification/data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/helenkilleen/Desktop/CODING/seabirds-northern-ecosystems/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{02F37982-1B61-A345-A6F1-CDB7853F3E90}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{164C7543-7070-1943-AE36-1B6D198E3A1C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-21600" yWindow="-7900" windowWidth="21600" windowHeight="38400" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -76,9 +76,6 @@
     <t>arctic tern_Foula</t>
   </si>
   <si>
-    <t>arctic tern_Matinicius Rock</t>
-  </si>
-  <si>
     <t>arctic tern_Seal Island NWR</t>
   </si>
   <si>
@@ -100,9 +97,6 @@
     <t>Atlantic puffin_Machias Seal</t>
   </si>
   <si>
-    <t>Atlantic puffin_Matinicius Rock</t>
-  </si>
-  <si>
     <t>Atlantic puffin_Papey</t>
   </si>
   <si>
@@ -241,9 +235,6 @@
     <t>common tern_Jenny</t>
   </si>
   <si>
-    <t>common tern_Matinicius Rock</t>
-  </si>
-  <si>
     <t>common tern_Outer Green</t>
   </si>
   <si>
@@ -644,6 +635,15 @@
   </si>
   <si>
     <t>black-legged kittiwake_Rost</t>
+  </si>
+  <si>
+    <t>arctic tern_Matinicus Rock</t>
+  </si>
+  <si>
+    <t>Atlantic puffin_Matinicus Rock</t>
+  </si>
+  <si>
+    <t>common tern_Matinicus Rock</t>
   </si>
 </sst>
 </file>
@@ -1508,8 +1508,8 @@
   <dimension ref="A1:L142"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="200" zoomScaleNormal="200" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A14" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A39" sqref="A39"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A9" sqref="A9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1530,34 +1530,34 @@
         <v>1</v>
       </c>
       <c r="C1" t="s">
+        <v>144</v>
+      </c>
+      <c r="D1" t="s">
+        <v>145</v>
+      </c>
+      <c r="E1" t="s">
+        <v>146</v>
+      </c>
+      <c r="F1" t="s">
         <v>147</v>
       </c>
-      <c r="D1" t="s">
-        <v>148</v>
-      </c>
-      <c r="E1" t="s">
-        <v>149</v>
-      </c>
-      <c r="F1" t="s">
-        <v>150</v>
-      </c>
       <c r="G1" t="s">
-        <v>170</v>
+        <v>167</v>
       </c>
       <c r="H1" t="s">
+        <v>168</v>
+      </c>
+      <c r="I1" t="s">
         <v>171</v>
       </c>
-      <c r="I1" t="s">
-        <v>174</v>
-      </c>
       <c r="J1" t="s">
-        <v>184</v>
+        <v>181</v>
       </c>
       <c r="K1" t="s">
-        <v>185</v>
+        <v>182</v>
       </c>
       <c r="L1" t="s">
-        <v>186</v>
+        <v>183</v>
       </c>
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.2">
@@ -1580,13 +1580,13 @@
         <v>7</v>
       </c>
       <c r="G2" t="s">
-        <v>162</v>
+        <v>159</v>
       </c>
       <c r="H2" t="s">
-        <v>173</v>
+        <v>170</v>
       </c>
       <c r="I2" t="s">
-        <v>199</v>
+        <v>196</v>
       </c>
       <c r="J2">
         <f>D2-C2</f>
@@ -1621,10 +1621,10 @@
         <v>7</v>
       </c>
       <c r="G3" t="s">
-        <v>165</v>
+        <v>162</v>
       </c>
       <c r="H3" s="6" t="s">
-        <v>173</v>
+        <v>170</v>
       </c>
       <c r="J3">
         <f t="shared" ref="J3:J64" si="0">D3-C3</f>
@@ -1659,7 +1659,7 @@
         <v>8</v>
       </c>
       <c r="I4" t="s">
-        <v>175</v>
+        <v>172</v>
       </c>
       <c r="J4">
         <f t="shared" si="0"/>
@@ -1694,7 +1694,7 @@
         <v>7</v>
       </c>
       <c r="H5" t="s">
-        <v>172</v>
+        <v>169</v>
       </c>
       <c r="J5">
         <f t="shared" si="0"/>
@@ -1729,10 +1729,10 @@
         <v>7</v>
       </c>
       <c r="H6" s="6" t="s">
-        <v>173</v>
+        <v>170</v>
       </c>
       <c r="I6" t="s">
-        <v>178</v>
+        <v>175</v>
       </c>
       <c r="J6">
         <f t="shared" si="0"/>
@@ -1767,10 +1767,10 @@
         <v>7</v>
       </c>
       <c r="H7" s="6" t="s">
-        <v>173</v>
+        <v>170</v>
       </c>
       <c r="I7" t="s">
-        <v>178</v>
+        <v>175</v>
       </c>
       <c r="J7">
         <f t="shared" si="0"/>
@@ -1805,13 +1805,13 @@
         <v>7</v>
       </c>
       <c r="G8" t="s">
-        <v>162</v>
+        <v>159</v>
       </c>
       <c r="H8" s="6" t="s">
-        <v>173</v>
+        <v>170</v>
       </c>
       <c r="I8" t="s">
-        <v>178</v>
+        <v>175</v>
       </c>
       <c r="J8">
         <f t="shared" si="0"/>
@@ -1828,7 +1828,7 @@
     </row>
     <row r="9" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>13</v>
+        <v>200</v>
       </c>
       <c r="B9" t="s">
         <v>10</v>
@@ -1846,10 +1846,10 @@
         <v>7</v>
       </c>
       <c r="H9" s="6" t="s">
-        <v>173</v>
+        <v>170</v>
       </c>
       <c r="I9" t="s">
-        <v>178</v>
+        <v>175</v>
       </c>
       <c r="J9">
         <f t="shared" si="0"/>
@@ -1866,7 +1866,7 @@
     </row>
     <row r="10" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B10" t="s">
         <v>10</v>
@@ -1884,10 +1884,10 @@
         <v>7</v>
       </c>
       <c r="H10" s="6" t="s">
-        <v>173</v>
+        <v>170</v>
       </c>
       <c r="I10" t="s">
-        <v>178</v>
+        <v>175</v>
       </c>
       <c r="J10">
         <f t="shared" si="0"/>
@@ -1904,7 +1904,7 @@
     </row>
     <row r="11" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B11" t="s">
         <v>7</v>
@@ -1922,13 +1922,13 @@
         <v>7</v>
       </c>
       <c r="G11" s="6" t="s">
-        <v>165</v>
+        <v>162</v>
       </c>
       <c r="H11" s="6" t="s">
-        <v>173</v>
+        <v>170</v>
       </c>
       <c r="I11" t="s">
-        <v>178</v>
+        <v>175</v>
       </c>
       <c r="J11">
         <f t="shared" si="0"/>
@@ -1945,7 +1945,7 @@
     </row>
     <row r="12" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B12" t="s">
         <v>3</v>
@@ -1963,7 +1963,7 @@
         <v>10</v>
       </c>
       <c r="H12" s="6" t="s">
-        <v>173</v>
+        <v>170</v>
       </c>
       <c r="J12">
         <f t="shared" si="0"/>
@@ -1980,7 +1980,7 @@
     </row>
     <row r="13" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B13" t="s">
         <v>7</v>
@@ -1998,7 +1998,7 @@
         <v>8</v>
       </c>
       <c r="G13" t="s">
-        <v>182</v>
+        <v>179</v>
       </c>
       <c r="J13">
         <f t="shared" si="0"/>
@@ -2015,10 +2015,10 @@
     </row>
     <row r="14" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>145</v>
+        <v>142</v>
       </c>
       <c r="B14" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C14">
         <v>4</v>
@@ -2033,7 +2033,7 @@
         <v>8</v>
       </c>
       <c r="G14" t="s">
-        <v>182</v>
+        <v>179</v>
       </c>
       <c r="J14">
         <f t="shared" si="0"/>
@@ -2050,7 +2050,7 @@
     </row>
     <row r="15" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
-        <v>146</v>
+        <v>143</v>
       </c>
       <c r="B15" t="s">
         <v>7</v>
@@ -2068,10 +2068,10 @@
         <v>8</v>
       </c>
       <c r="H15" s="6" t="s">
-        <v>172</v>
+        <v>169</v>
       </c>
       <c r="I15" t="s">
-        <v>177</v>
+        <v>174</v>
       </c>
       <c r="J15">
         <f t="shared" si="0"/>
@@ -2088,7 +2088,7 @@
     </row>
     <row r="16" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B16" t="s">
         <v>7</v>
@@ -2120,7 +2120,7 @@
     </row>
     <row r="17" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B17" t="s">
         <v>10</v>
@@ -2138,7 +2138,7 @@
         <v>7</v>
       </c>
       <c r="I17" s="6" t="s">
-        <v>178</v>
+        <v>175</v>
       </c>
       <c r="J17">
         <f t="shared" si="0"/>
@@ -2155,7 +2155,7 @@
     </row>
     <row r="18" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
-        <v>21</v>
+        <v>201</v>
       </c>
       <c r="B18" t="s">
         <v>10</v>
@@ -2173,7 +2173,7 @@
         <v>7</v>
       </c>
       <c r="I18" s="6" t="s">
-        <v>178</v>
+        <v>175</v>
       </c>
       <c r="J18">
         <f t="shared" si="0"/>
@@ -2190,10 +2190,10 @@
     </row>
     <row r="19" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="B19" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C19">
         <v>4</v>
@@ -2208,7 +2208,7 @@
         <v>8</v>
       </c>
       <c r="G19" t="s">
-        <v>182</v>
+        <v>179</v>
       </c>
       <c r="J19">
         <f t="shared" si="0"/>
@@ -2225,7 +2225,7 @@
     </row>
     <row r="20" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="B20" t="s">
         <v>7</v>
@@ -2243,7 +2243,7 @@
         <v>8</v>
       </c>
       <c r="G20" t="s">
-        <v>166</v>
+        <v>163</v>
       </c>
       <c r="J20">
         <f t="shared" si="0"/>
@@ -2260,7 +2260,7 @@
     </row>
     <row r="21" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="B21" t="s">
         <v>10</v>
@@ -2278,10 +2278,10 @@
         <v>7</v>
       </c>
       <c r="G21" t="s">
-        <v>183</v>
+        <v>180</v>
       </c>
       <c r="I21" s="6" t="s">
-        <v>178</v>
+        <v>175</v>
       </c>
       <c r="J21">
         <f t="shared" si="0"/>
@@ -2298,7 +2298,7 @@
     </row>
     <row r="22" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="B22" t="s">
         <v>7</v>
@@ -2316,7 +2316,7 @@
         <v>8</v>
       </c>
       <c r="G22" t="s">
-        <v>182</v>
+        <v>179</v>
       </c>
       <c r="J22">
         <f t="shared" si="0"/>
@@ -2333,10 +2333,10 @@
     </row>
     <row r="23" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="B23" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="C23">
         <v>2</v>
@@ -2351,7 +2351,7 @@
         <v>7</v>
       </c>
       <c r="G23" t="s">
-        <v>179</v>
+        <v>176</v>
       </c>
       <c r="J23">
         <f t="shared" si="0"/>
@@ -2368,10 +2368,10 @@
     </row>
     <row r="24" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="B24" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="C24">
         <v>8</v>
@@ -2386,10 +2386,10 @@
         <v>4</v>
       </c>
       <c r="G24" t="s">
-        <v>153</v>
+        <v>150</v>
       </c>
       <c r="H24" s="6" t="s">
-        <v>173</v>
+        <v>170</v>
       </c>
       <c r="J24">
         <f t="shared" si="0"/>
@@ -2406,10 +2406,10 @@
     </row>
     <row r="25" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="B25" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="C25">
         <v>8</v>
@@ -2424,10 +2424,10 @@
         <v>4</v>
       </c>
       <c r="G25" t="s">
-        <v>153</v>
+        <v>150</v>
       </c>
       <c r="H25" s="6" t="s">
-        <v>173</v>
+        <v>170</v>
       </c>
       <c r="J25">
         <f t="shared" si="0"/>
@@ -2444,7 +2444,7 @@
     </row>
     <row r="26" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="B26" t="s">
         <v>3</v>
@@ -2462,13 +2462,13 @@
         <v>8</v>
       </c>
       <c r="G26" s="6" t="s">
-        <v>165</v>
+        <v>162</v>
       </c>
       <c r="H26" s="6" t="s">
-        <v>173</v>
+        <v>170</v>
       </c>
       <c r="I26" s="6" t="s">
-        <v>175</v>
+        <v>172</v>
       </c>
       <c r="J26">
         <f t="shared" si="0"/>
@@ -2485,10 +2485,10 @@
     </row>
     <row r="27" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="B27" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C27">
         <v>4</v>
@@ -2503,10 +2503,10 @@
         <v>9</v>
       </c>
       <c r="G27" s="6" t="s">
-        <v>162</v>
+        <v>159</v>
       </c>
       <c r="H27" s="6" t="s">
-        <v>173</v>
+        <v>170</v>
       </c>
       <c r="J27">
         <f t="shared" si="0"/>
@@ -2523,10 +2523,10 @@
     </row>
     <row r="28" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="B28" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C28">
         <v>3</v>
@@ -2541,13 +2541,13 @@
         <v>8</v>
       </c>
       <c r="G28" s="6" t="s">
-        <v>162</v>
+        <v>159</v>
       </c>
       <c r="H28" s="6" t="s">
-        <v>173</v>
+        <v>170</v>
       </c>
       <c r="I28" s="6" t="s">
-        <v>175</v>
+        <v>172</v>
       </c>
       <c r="J28">
         <f t="shared" si="0"/>
@@ -2564,7 +2564,7 @@
     </row>
     <row r="29" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="B29" t="s">
         <v>3</v>
@@ -2582,10 +2582,10 @@
         <v>8</v>
       </c>
       <c r="G29" s="6" t="s">
-        <v>162</v>
+        <v>159</v>
       </c>
       <c r="H29" s="6" t="s">
-        <v>173</v>
+        <v>170</v>
       </c>
       <c r="J29">
         <f t="shared" si="0"/>
@@ -2602,7 +2602,7 @@
     </row>
     <row r="30" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="B30" t="s">
         <v>3</v>
@@ -2620,13 +2620,13 @@
         <v>8</v>
       </c>
       <c r="G30" s="6" t="s">
-        <v>162</v>
+        <v>159</v>
       </c>
       <c r="H30" s="6" t="s">
-        <v>173</v>
+        <v>170</v>
       </c>
       <c r="I30" s="6" t="s">
-        <v>175</v>
+        <v>172</v>
       </c>
       <c r="J30">
         <f t="shared" si="0"/>
@@ -2643,7 +2643,7 @@
     </row>
     <row r="31" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="B31" t="s">
         <v>7</v>
@@ -2661,10 +2661,10 @@
         <v>7</v>
       </c>
       <c r="G31" s="6" t="s">
-        <v>165</v>
+        <v>162</v>
       </c>
       <c r="H31" s="6" t="s">
-        <v>172</v>
+        <v>169</v>
       </c>
       <c r="J31">
         <f t="shared" si="0"/>
@@ -2681,7 +2681,7 @@
     </row>
     <row r="32" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="B32" t="s">
         <v>7</v>
@@ -2713,7 +2713,7 @@
     </row>
     <row r="33" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="B33" t="s">
         <v>3</v>
@@ -2731,10 +2731,10 @@
         <v>8</v>
       </c>
       <c r="G33" t="s">
-        <v>154</v>
+        <v>151</v>
       </c>
       <c r="H33" s="6" t="s">
-        <v>173</v>
+        <v>170</v>
       </c>
       <c r="J33">
         <f t="shared" si="0"/>
@@ -2751,7 +2751,7 @@
     </row>
     <row r="34" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="B34" t="s">
         <v>7</v>
@@ -2769,10 +2769,10 @@
         <v>7</v>
       </c>
       <c r="H34" s="6" t="s">
+        <v>169</v>
+      </c>
+      <c r="I34" s="6" t="s">
         <v>172</v>
-      </c>
-      <c r="I34" s="6" t="s">
-        <v>175</v>
       </c>
       <c r="J34">
         <f t="shared" si="0"/>
@@ -2789,10 +2789,10 @@
     </row>
     <row r="35" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="B35" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C35">
         <v>3</v>
@@ -2807,13 +2807,13 @@
         <v>8</v>
       </c>
       <c r="G35" s="6" t="s">
-        <v>162</v>
+        <v>159</v>
       </c>
       <c r="H35" s="6" t="s">
-        <v>173</v>
+        <v>170</v>
       </c>
       <c r="I35" s="6" t="s">
-        <v>175</v>
+        <v>172</v>
       </c>
       <c r="J35">
         <f t="shared" si="0"/>
@@ -2830,10 +2830,10 @@
     </row>
     <row r="36" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="B36" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C36">
         <v>3</v>
@@ -2848,13 +2848,13 @@
         <v>8</v>
       </c>
       <c r="G36" s="6" t="s">
-        <v>162</v>
+        <v>159</v>
       </c>
       <c r="H36" s="6" t="s">
-        <v>173</v>
+        <v>170</v>
       </c>
       <c r="I36" s="6" t="s">
-        <v>175</v>
+        <v>172</v>
       </c>
       <c r="J36">
         <f t="shared" si="0"/>
@@ -2871,7 +2871,7 @@
     </row>
     <row r="37" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="B37" t="s">
         <v>5</v>
@@ -2889,13 +2889,13 @@
         <v>8</v>
       </c>
       <c r="G37" t="s">
-        <v>167</v>
+        <v>164</v>
       </c>
       <c r="H37" s="6" t="s">
-        <v>173</v>
+        <v>170</v>
       </c>
       <c r="I37" s="6" t="s">
-        <v>175</v>
+        <v>172</v>
       </c>
       <c r="J37">
         <f t="shared" si="0"/>
@@ -2912,7 +2912,7 @@
     </row>
     <row r="38" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
-        <v>202</v>
+        <v>199</v>
       </c>
       <c r="B38" t="s">
         <v>7</v>
@@ -2930,10 +2930,10 @@
         <v>6</v>
       </c>
       <c r="H38" s="6" t="s">
+        <v>169</v>
+      </c>
+      <c r="I38" s="6" t="s">
         <v>172</v>
-      </c>
-      <c r="I38" s="6" t="s">
-        <v>175</v>
       </c>
       <c r="J38">
         <f t="shared" si="0"/>
@@ -2950,7 +2950,7 @@
     </row>
     <row r="39" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
-        <v>201</v>
+        <v>198</v>
       </c>
       <c r="B39" t="s">
         <v>7</v>
@@ -2968,7 +2968,7 @@
         <v>7</v>
       </c>
       <c r="G39" t="s">
-        <v>169</v>
+        <v>166</v>
       </c>
       <c r="J39">
         <f t="shared" si="0"/>
@@ -2985,7 +2985,7 @@
     </row>
     <row r="40" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="B40" t="s">
         <v>5</v>
@@ -3003,7 +3003,7 @@
         <v>8</v>
       </c>
       <c r="G40" t="s">
-        <v>180</v>
+        <v>177</v>
       </c>
       <c r="J40">
         <f t="shared" si="0"/>
@@ -3020,7 +3020,7 @@
     </row>
     <row r="41" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="B41" t="s">
         <v>3</v>
@@ -3038,7 +3038,7 @@
         <v>8</v>
       </c>
       <c r="G41" t="s">
-        <v>155</v>
+        <v>152</v>
       </c>
       <c r="J41">
         <f t="shared" si="0"/>
@@ -3055,7 +3055,7 @@
     </row>
     <row r="42" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="B42" t="s">
         <v>3</v>
@@ -3073,7 +3073,7 @@
         <v>8</v>
       </c>
       <c r="I42" s="6" t="s">
-        <v>175</v>
+        <v>172</v>
       </c>
       <c r="J42">
         <f t="shared" si="0"/>
@@ -3090,7 +3090,7 @@
     </row>
     <row r="43" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="B43" t="s">
         <v>3</v>
@@ -3108,13 +3108,13 @@
         <v>9</v>
       </c>
       <c r="G43" s="6" t="s">
-        <v>162</v>
+        <v>159</v>
       </c>
       <c r="H43" s="6" t="s">
+        <v>169</v>
+      </c>
+      <c r="I43" s="6" t="s">
         <v>172</v>
-      </c>
-      <c r="I43" s="6" t="s">
-        <v>175</v>
       </c>
       <c r="J43">
         <f t="shared" si="0"/>
@@ -3131,10 +3131,10 @@
     </row>
     <row r="44" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A44" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="B44" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="C44">
         <v>1</v>
@@ -3149,7 +3149,7 @@
         <v>7</v>
       </c>
       <c r="H44" s="6" t="s">
-        <v>172</v>
+        <v>169</v>
       </c>
       <c r="J44">
         <f t="shared" si="0"/>
@@ -3166,10 +3166,10 @@
     </row>
     <row r="45" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A45" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="B45" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="C45">
         <v>1</v>
@@ -3184,7 +3184,7 @@
         <v>7</v>
       </c>
       <c r="I45" s="6" t="s">
-        <v>175</v>
+        <v>172</v>
       </c>
       <c r="J45">
         <f t="shared" si="0"/>
@@ -3201,7 +3201,7 @@
     </row>
     <row r="46" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A46" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="B46" t="s">
         <v>3</v>
@@ -3219,10 +3219,10 @@
         <v>9</v>
       </c>
       <c r="G46" t="s">
-        <v>153</v>
+        <v>150</v>
       </c>
       <c r="H46" s="6" t="s">
-        <v>173</v>
+        <v>170</v>
       </c>
       <c r="J46">
         <f t="shared" si="0"/>
@@ -3239,7 +3239,7 @@
     </row>
     <row r="47" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A47" t="s">
-        <v>156</v>
+        <v>153</v>
       </c>
       <c r="B47" t="s">
         <v>3</v>
@@ -3257,10 +3257,10 @@
         <v>9</v>
       </c>
       <c r="H47" s="6" t="s">
-        <v>173</v>
+        <v>170</v>
       </c>
       <c r="I47" s="6" t="s">
-        <v>175</v>
+        <v>172</v>
       </c>
       <c r="J47">
         <f t="shared" si="0"/>
@@ -3277,7 +3277,7 @@
     </row>
     <row r="48" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A48" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="B48" t="s">
         <v>3</v>
@@ -3295,13 +3295,13 @@
         <v>9</v>
       </c>
       <c r="G48" s="6" t="s">
-        <v>162</v>
+        <v>159</v>
       </c>
       <c r="H48" s="6" t="s">
-        <v>173</v>
+        <v>170</v>
       </c>
       <c r="I48" s="6" t="s">
-        <v>175</v>
+        <v>172</v>
       </c>
       <c r="J48">
         <f t="shared" si="0"/>
@@ -3318,10 +3318,10 @@
     </row>
     <row r="49" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A49" t="s">
-        <v>164</v>
+        <v>161</v>
       </c>
       <c r="B49" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C49">
         <v>3</v>
@@ -3336,13 +3336,13 @@
         <v>8</v>
       </c>
       <c r="G49" t="s">
-        <v>162</v>
+        <v>159</v>
       </c>
       <c r="H49" s="6" t="s">
-        <v>173</v>
+        <v>170</v>
       </c>
       <c r="I49" s="6" t="s">
-        <v>175</v>
+        <v>172</v>
       </c>
       <c r="J49">
         <f t="shared" si="0"/>
@@ -3359,7 +3359,7 @@
     </row>
     <row r="50" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A50" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="B50" t="s">
         <v>3</v>
@@ -3377,10 +3377,10 @@
         <v>8</v>
       </c>
       <c r="G50" s="6" t="s">
-        <v>162</v>
+        <v>159</v>
       </c>
       <c r="H50" s="6" t="s">
-        <v>173</v>
+        <v>170</v>
       </c>
       <c r="J50">
         <f t="shared" si="0"/>
@@ -3397,10 +3397,10 @@
     </row>
     <row r="51" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A51" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="B51" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C51">
         <v>3</v>
@@ -3415,13 +3415,13 @@
         <v>8</v>
       </c>
       <c r="G51" s="6" t="s">
-        <v>162</v>
+        <v>159</v>
       </c>
       <c r="H51" s="6" t="s">
-        <v>173</v>
+        <v>170</v>
       </c>
       <c r="I51" s="6" t="s">
-        <v>175</v>
+        <v>172</v>
       </c>
       <c r="J51">
         <f t="shared" si="0"/>
@@ -3438,7 +3438,7 @@
     </row>
     <row r="52" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A52" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="B52" t="s">
         <v>3</v>
@@ -3456,13 +3456,13 @@
         <v>8</v>
       </c>
       <c r="G52" s="6" t="s">
-        <v>162</v>
+        <v>159</v>
       </c>
       <c r="H52" s="6" t="s">
-        <v>173</v>
+        <v>170</v>
       </c>
       <c r="I52" s="6" t="s">
-        <v>175</v>
+        <v>172</v>
       </c>
       <c r="J52">
         <f t="shared" si="0"/>
@@ -3479,7 +3479,7 @@
     </row>
     <row r="53" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A53" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="B53" t="s">
         <v>3</v>
@@ -3497,13 +3497,13 @@
         <v>9</v>
       </c>
       <c r="G53" s="6" t="s">
-        <v>162</v>
+        <v>159</v>
       </c>
       <c r="H53" s="6" t="s">
-        <v>173</v>
+        <v>170</v>
       </c>
       <c r="I53" s="6" t="s">
-        <v>175</v>
+        <v>172</v>
       </c>
       <c r="J53">
         <f t="shared" si="0"/>
@@ -3520,7 +3520,7 @@
     </row>
     <row r="54" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A54" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="B54" t="s">
         <v>7</v>
@@ -3538,7 +3538,7 @@
         <v>7</v>
       </c>
       <c r="H54" s="6" t="s">
-        <v>173</v>
+        <v>170</v>
       </c>
       <c r="J54">
         <f t="shared" si="0"/>
@@ -3555,7 +3555,7 @@
     </row>
     <row r="55" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A55" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="B55" t="s">
         <v>7</v>
@@ -3573,10 +3573,10 @@
         <v>7</v>
       </c>
       <c r="G55" s="6" t="s">
-        <v>166</v>
+        <v>163</v>
       </c>
       <c r="H55" s="6" t="s">
-        <v>173</v>
+        <v>170</v>
       </c>
       <c r="J55">
         <f t="shared" si="0"/>
@@ -3593,7 +3593,7 @@
     </row>
     <row r="56" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A56" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="B56" t="s">
         <v>3</v>
@@ -3611,10 +3611,10 @@
         <v>7</v>
       </c>
       <c r="H56" s="6" t="s">
-        <v>173</v>
+        <v>170</v>
       </c>
       <c r="I56" s="6" t="s">
-        <v>175</v>
+        <v>172</v>
       </c>
       <c r="J56">
         <f t="shared" si="0"/>
@@ -3631,7 +3631,7 @@
     </row>
     <row r="57" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A57" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="B57" t="s">
         <v>7</v>
@@ -3649,7 +3649,7 @@
         <v>7</v>
       </c>
       <c r="H57" s="6" t="s">
-        <v>173</v>
+        <v>170</v>
       </c>
       <c r="J57">
         <f t="shared" si="0"/>
@@ -3666,10 +3666,10 @@
     </row>
     <row r="58" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A58" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="B58" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C58">
         <v>4</v>
@@ -3684,13 +3684,13 @@
         <v>9</v>
       </c>
       <c r="G58" s="6" t="s">
-        <v>162</v>
+        <v>159</v>
       </c>
       <c r="H58" s="6" t="s">
-        <v>173</v>
+        <v>170</v>
       </c>
       <c r="I58" s="6" t="s">
-        <v>175</v>
+        <v>172</v>
       </c>
       <c r="J58">
         <f t="shared" si="0"/>
@@ -3707,7 +3707,7 @@
     </row>
     <row r="59" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A59" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="B59" t="s">
         <v>3</v>
@@ -3725,10 +3725,10 @@
         <v>8</v>
       </c>
       <c r="G59" s="6" t="s">
-        <v>162</v>
+        <v>159</v>
       </c>
       <c r="H59" s="6" t="s">
-        <v>173</v>
+        <v>170</v>
       </c>
       <c r="J59">
         <f t="shared" si="0"/>
@@ -3745,10 +3745,10 @@
     </row>
     <row r="60" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A60" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="B60" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C60">
         <v>4</v>
@@ -3763,10 +3763,10 @@
         <v>8</v>
       </c>
       <c r="G60" s="6" t="s">
-        <v>162</v>
+        <v>159</v>
       </c>
       <c r="H60" s="6" t="s">
-        <v>173</v>
+        <v>170</v>
       </c>
       <c r="J60">
         <f t="shared" si="0"/>
@@ -3783,7 +3783,7 @@
     </row>
     <row r="61" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A61" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="B61" t="s">
         <v>5</v>
@@ -3801,10 +3801,10 @@
         <v>8</v>
       </c>
       <c r="G61" s="6" t="s">
-        <v>166</v>
+        <v>163</v>
       </c>
       <c r="H61" s="6" t="s">
-        <v>173</v>
+        <v>170</v>
       </c>
       <c r="J61">
         <f t="shared" si="0"/>
@@ -3821,7 +3821,7 @@
     </row>
     <row r="62" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A62" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="B62" t="s">
         <v>3</v>
@@ -3839,13 +3839,13 @@
         <v>8</v>
       </c>
       <c r="G62" s="6" t="s">
-        <v>162</v>
+        <v>159</v>
       </c>
       <c r="H62" s="6" t="s">
-        <v>173</v>
+        <v>170</v>
       </c>
       <c r="I62" s="6" t="s">
-        <v>175</v>
+        <v>172</v>
       </c>
       <c r="J62">
         <f t="shared" si="0"/>
@@ -3862,7 +3862,7 @@
     </row>
     <row r="63" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A63" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="B63" t="s">
         <v>10</v>
@@ -3880,13 +3880,13 @@
         <v>7</v>
       </c>
       <c r="G63" s="6" t="s">
-        <v>165</v>
+        <v>162</v>
       </c>
       <c r="H63" s="6" t="s">
-        <v>173</v>
+        <v>170</v>
       </c>
       <c r="I63" s="6" t="s">
-        <v>178</v>
+        <v>175</v>
       </c>
       <c r="J63">
         <f t="shared" si="0"/>
@@ -3903,7 +3903,7 @@
     </row>
     <row r="64" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A64" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="B64" t="s">
         <v>10</v>
@@ -3921,13 +3921,13 @@
         <v>7</v>
       </c>
       <c r="G64" s="6" t="s">
-        <v>162</v>
+        <v>159</v>
       </c>
       <c r="H64" s="6" t="s">
-        <v>173</v>
+        <v>170</v>
       </c>
       <c r="I64" s="6" t="s">
-        <v>178</v>
+        <v>175</v>
       </c>
       <c r="J64">
         <f t="shared" si="0"/>
@@ -3944,7 +3944,7 @@
     </row>
     <row r="65" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A65" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="B65" t="s">
         <v>10</v>
@@ -3962,13 +3962,13 @@
         <v>7</v>
       </c>
       <c r="G65" s="6" t="s">
-        <v>162</v>
+        <v>159</v>
       </c>
       <c r="H65" s="6" t="s">
-        <v>173</v>
+        <v>170</v>
       </c>
       <c r="I65" s="6" t="s">
-        <v>178</v>
+        <v>175</v>
       </c>
       <c r="J65">
         <f t="shared" ref="J65:J128" si="3">D65-C65</f>
@@ -3985,7 +3985,7 @@
     </row>
     <row r="66" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A66" t="s">
-        <v>68</v>
+        <v>202</v>
       </c>
       <c r="B66" t="s">
         <v>10</v>
@@ -4003,13 +4003,13 @@
         <v>7</v>
       </c>
       <c r="G66" s="6" t="s">
-        <v>165</v>
+        <v>162</v>
       </c>
       <c r="H66" s="6" t="s">
-        <v>173</v>
+        <v>170</v>
       </c>
       <c r="I66" s="6" t="s">
-        <v>178</v>
+        <v>175</v>
       </c>
       <c r="J66">
         <f t="shared" si="3"/>
@@ -4026,7 +4026,7 @@
     </row>
     <row r="67" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A67" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="B67" t="s">
         <v>10</v>
@@ -4044,10 +4044,10 @@
         <v>7</v>
       </c>
       <c r="H67" s="6" t="s">
-        <v>173</v>
+        <v>170</v>
       </c>
       <c r="I67" s="6" t="s">
-        <v>178</v>
+        <v>175</v>
       </c>
       <c r="J67">
         <f t="shared" si="3"/>
@@ -4064,7 +4064,7 @@
     </row>
     <row r="68" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A68" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
       <c r="B68" t="s">
         <v>10</v>
@@ -4082,13 +4082,13 @@
         <v>7</v>
       </c>
       <c r="G68" s="6" t="s">
-        <v>165</v>
+        <v>162</v>
       </c>
       <c r="H68" s="6" t="s">
-        <v>173</v>
+        <v>170</v>
       </c>
       <c r="I68" s="6" t="s">
-        <v>178</v>
+        <v>175</v>
       </c>
       <c r="J68">
         <f t="shared" si="3"/>
@@ -4105,7 +4105,7 @@
     </row>
     <row r="69" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A69" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="B69" t="s">
         <v>10</v>
@@ -4123,13 +4123,13 @@
         <v>7</v>
       </c>
       <c r="G69" s="6" t="s">
-        <v>162</v>
+        <v>159</v>
       </c>
       <c r="H69" s="6" t="s">
-        <v>173</v>
+        <v>170</v>
       </c>
       <c r="I69" s="6" t="s">
-        <v>178</v>
+        <v>175</v>
       </c>
       <c r="J69">
         <f t="shared" si="3"/>
@@ -4146,7 +4146,7 @@
     </row>
     <row r="70" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A70" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="B70" t="s">
         <v>10</v>
@@ -4164,13 +4164,13 @@
         <v>7</v>
       </c>
       <c r="G70" s="6" t="s">
-        <v>162</v>
+        <v>159</v>
       </c>
       <c r="H70" s="6" t="s">
-        <v>173</v>
+        <v>170</v>
       </c>
       <c r="I70" s="6" t="s">
-        <v>178</v>
+        <v>175</v>
       </c>
       <c r="J70">
         <f t="shared" si="3"/>
@@ -4187,7 +4187,7 @@
     </row>
     <row r="71" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A71" t="s">
-        <v>200</v>
+        <v>197</v>
       </c>
       <c r="B71" t="s">
         <v>7</v>
@@ -4205,7 +4205,7 @@
         <v>7</v>
       </c>
       <c r="G71" s="6" t="s">
-        <v>181</v>
+        <v>178</v>
       </c>
       <c r="J71">
         <f t="shared" si="3"/>
@@ -4222,7 +4222,7 @@
     </row>
     <row r="72" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A72" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="B72" t="s">
         <v>3</v>
@@ -4240,10 +4240,10 @@
         <v>7</v>
       </c>
       <c r="G72" s="6" t="s">
-        <v>162</v>
+        <v>159</v>
       </c>
       <c r="H72" s="6" t="s">
-        <v>173</v>
+        <v>170</v>
       </c>
       <c r="J72">
         <f t="shared" si="3"/>
@@ -4260,7 +4260,7 @@
     </row>
     <row r="73" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A73" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="B73" t="s">
         <v>5</v>
@@ -4278,10 +4278,10 @@
         <v>7</v>
       </c>
       <c r="G73" s="6" t="s">
-        <v>166</v>
+        <v>163</v>
       </c>
       <c r="H73" s="6" t="s">
-        <v>173</v>
+        <v>170</v>
       </c>
       <c r="J73">
         <f t="shared" si="3"/>
@@ -4298,7 +4298,7 @@
     </row>
     <row r="74" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A74" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="B74" t="s">
         <v>3</v>
@@ -4330,7 +4330,7 @@
     </row>
     <row r="75" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A75" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="B75" t="s">
         <v>7</v>
@@ -4348,7 +4348,7 @@
         <v>7</v>
       </c>
       <c r="H75" s="6" t="s">
-        <v>173</v>
+        <v>170</v>
       </c>
       <c r="J75">
         <f t="shared" si="3"/>
@@ -4365,7 +4365,7 @@
     </row>
     <row r="76" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A76" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="B76" t="s">
         <v>7</v>
@@ -4383,10 +4383,10 @@
         <v>7</v>
       </c>
       <c r="H76" s="6" t="s">
-        <v>173</v>
+        <v>170</v>
       </c>
       <c r="I76" t="s">
-        <v>175</v>
+        <v>172</v>
       </c>
       <c r="J76">
         <f t="shared" si="3"/>
@@ -4403,7 +4403,7 @@
     </row>
     <row r="77" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A77" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="B77" t="s">
         <v>7</v>
@@ -4421,10 +4421,10 @@
         <v>7</v>
       </c>
       <c r="H77" s="6" t="s">
-        <v>173</v>
+        <v>170</v>
       </c>
       <c r="I77" s="6" t="s">
-        <v>175</v>
+        <v>172</v>
       </c>
       <c r="J77">
         <f t="shared" si="3"/>
@@ -4441,7 +4441,7 @@
     </row>
     <row r="78" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A78" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="B78" t="s">
         <v>7</v>
@@ -4459,10 +4459,10 @@
         <v>8</v>
       </c>
       <c r="H78" s="6" t="s">
-        <v>173</v>
+        <v>170</v>
       </c>
       <c r="I78" s="6" t="s">
-        <v>175</v>
+        <v>172</v>
       </c>
       <c r="J78">
         <f t="shared" si="3"/>
@@ -4479,7 +4479,7 @@
     </row>
     <row r="79" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A79" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
       <c r="B79" t="s">
         <v>3</v>
@@ -4497,13 +4497,13 @@
         <v>8</v>
       </c>
       <c r="G79" t="s">
-        <v>163</v>
+        <v>160</v>
       </c>
       <c r="H79" s="6" t="s">
-        <v>173</v>
+        <v>170</v>
       </c>
       <c r="I79" s="6" t="s">
-        <v>175</v>
+        <v>172</v>
       </c>
       <c r="J79">
         <f t="shared" si="3"/>
@@ -4520,7 +4520,7 @@
     </row>
     <row r="80" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A80" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="B80" t="s">
         <v>3</v>
@@ -4538,10 +4538,10 @@
         <v>8</v>
       </c>
       <c r="G80" t="s">
-        <v>163</v>
+        <v>160</v>
       </c>
       <c r="H80" s="6" t="s">
-        <v>173</v>
+        <v>170</v>
       </c>
       <c r="J80">
         <f t="shared" si="3"/>
@@ -4558,7 +4558,7 @@
     </row>
     <row r="81" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A81" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="B81" t="s">
         <v>3</v>
@@ -4576,10 +4576,10 @@
         <v>8</v>
       </c>
       <c r="G81" t="s">
-        <v>163</v>
+        <v>160</v>
       </c>
       <c r="H81" s="6" t="s">
-        <v>173</v>
+        <v>170</v>
       </c>
       <c r="J81">
         <f t="shared" si="3"/>
@@ -4596,7 +4596,7 @@
     </row>
     <row r="82" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A82" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
       <c r="B82" t="s">
         <v>3</v>
@@ -4614,13 +4614,13 @@
         <v>8</v>
       </c>
       <c r="G82" s="6" t="s">
-        <v>162</v>
+        <v>159</v>
       </c>
       <c r="H82" s="6" t="s">
-        <v>173</v>
+        <v>170</v>
       </c>
       <c r="I82" s="6" t="s">
-        <v>178</v>
+        <v>175</v>
       </c>
       <c r="J82">
         <f t="shared" si="3"/>
@@ -4637,7 +4637,7 @@
     </row>
     <row r="83" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A83" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
       <c r="B83" t="s">
         <v>3</v>
@@ -4655,13 +4655,13 @@
         <v>8</v>
       </c>
       <c r="G83" s="6" t="s">
-        <v>162</v>
+        <v>159</v>
       </c>
       <c r="H83" s="6" t="s">
-        <v>173</v>
+        <v>170</v>
       </c>
       <c r="I83" s="6" t="s">
-        <v>178</v>
+        <v>175</v>
       </c>
       <c r="J83">
         <f t="shared" si="3"/>
@@ -4678,7 +4678,7 @@
     </row>
     <row r="84" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A84" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
       <c r="B84" t="s">
         <v>3</v>
@@ -4696,13 +4696,13 @@
         <v>8</v>
       </c>
       <c r="G84" s="6" t="s">
-        <v>162</v>
+        <v>159</v>
       </c>
       <c r="H84" s="6" t="s">
-        <v>173</v>
+        <v>170</v>
       </c>
       <c r="I84" s="6" t="s">
-        <v>178</v>
+        <v>175</v>
       </c>
       <c r="J84">
         <f t="shared" si="3"/>
@@ -4719,7 +4719,7 @@
     </row>
     <row r="85" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A85" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
       <c r="B85" t="s">
         <v>7</v>
@@ -4737,10 +4737,10 @@
         <v>8</v>
       </c>
       <c r="G85" s="6" t="s">
-        <v>196</v>
+        <v>193</v>
       </c>
       <c r="H85" s="6" t="s">
-        <v>173</v>
+        <v>170</v>
       </c>
       <c r="J85">
         <f t="shared" si="3"/>
@@ -4757,10 +4757,10 @@
     </row>
     <row r="86" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A86" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
       <c r="B86" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="C86">
         <v>2</v>
@@ -4775,7 +4775,7 @@
         <v>7</v>
       </c>
       <c r="I86" s="6" t="s">
-        <v>178</v>
+        <v>175</v>
       </c>
       <c r="J86">
         <f t="shared" si="3"/>
@@ -4792,7 +4792,7 @@
     </row>
     <row r="87" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A87" t="s">
-        <v>88</v>
+        <v>85</v>
       </c>
       <c r="B87" t="s">
         <v>3</v>
@@ -4810,13 +4810,13 @@
         <v>9</v>
       </c>
       <c r="G87" s="6" t="s">
-        <v>162</v>
+        <v>159</v>
       </c>
       <c r="H87" s="6" t="s">
-        <v>173</v>
+        <v>170</v>
       </c>
       <c r="I87" s="6" t="s">
-        <v>175</v>
+        <v>172</v>
       </c>
       <c r="J87">
         <f t="shared" si="3"/>
@@ -4833,7 +4833,7 @@
     </row>
     <row r="88" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A88" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
       <c r="B88" t="s">
         <v>3</v>
@@ -4851,10 +4851,10 @@
         <v>9</v>
       </c>
       <c r="G88" s="6" t="s">
-        <v>162</v>
+        <v>159</v>
       </c>
       <c r="H88" s="6" t="s">
-        <v>173</v>
+        <v>170</v>
       </c>
       <c r="J88">
         <f t="shared" si="3"/>
@@ -4871,7 +4871,7 @@
     </row>
     <row r="89" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A89" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
       <c r="B89" t="s">
         <v>3</v>
@@ -4889,10 +4889,10 @@
         <v>9</v>
       </c>
       <c r="G89" s="6" t="s">
-        <v>162</v>
+        <v>159</v>
       </c>
       <c r="H89" s="6" t="s">
-        <v>173</v>
+        <v>170</v>
       </c>
       <c r="J89">
         <f t="shared" si="3"/>
@@ -4909,7 +4909,7 @@
     </row>
     <row r="90" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A90" t="s">
-        <v>91</v>
+        <v>88</v>
       </c>
       <c r="B90" t="s">
         <v>5</v>
@@ -4927,10 +4927,10 @@
         <v>9</v>
       </c>
       <c r="G90" s="6" t="s">
-        <v>166</v>
+        <v>163</v>
       </c>
       <c r="H90" s="6" t="s">
-        <v>173</v>
+        <v>170</v>
       </c>
       <c r="J90">
         <f t="shared" si="3"/>
@@ -4947,7 +4947,7 @@
     </row>
     <row r="91" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A91" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
       <c r="B91" t="s">
         <v>5</v>
@@ -4965,10 +4965,10 @@
         <v>8</v>
       </c>
       <c r="G91" s="6" t="s">
-        <v>197</v>
+        <v>194</v>
       </c>
       <c r="H91" s="6" t="s">
-        <v>198</v>
+        <v>195</v>
       </c>
       <c r="J91">
         <f t="shared" si="3"/>
@@ -4985,10 +4985,10 @@
     </row>
     <row r="92" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A92" t="s">
-        <v>93</v>
+        <v>90</v>
       </c>
       <c r="B92" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="C92">
         <v>11</v>
@@ -5003,7 +5003,7 @@
         <v>5</v>
       </c>
       <c r="G92" t="s">
-        <v>157</v>
+        <v>154</v>
       </c>
       <c r="J92">
         <f t="shared" si="3"/>
@@ -5020,10 +5020,10 @@
     </row>
     <row r="93" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A93" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="B93" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="C93">
         <v>11</v>
@@ -5038,7 +5038,7 @@
         <v>5</v>
       </c>
       <c r="G93" t="s">
-        <v>157</v>
+        <v>154</v>
       </c>
       <c r="J93">
         <f t="shared" si="3"/>
@@ -5055,10 +5055,10 @@
     </row>
     <row r="94" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A94" t="s">
-        <v>95</v>
+        <v>92</v>
       </c>
       <c r="B94" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="C94">
         <v>11</v>
@@ -5073,7 +5073,7 @@
         <v>5</v>
       </c>
       <c r="G94" t="s">
-        <v>157</v>
+        <v>154</v>
       </c>
       <c r="J94">
         <f t="shared" si="3"/>
@@ -5090,7 +5090,7 @@
     </row>
     <row r="95" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A95" t="s">
-        <v>96</v>
+        <v>93</v>
       </c>
       <c r="B95" t="s">
         <v>3</v>
@@ -5108,13 +5108,13 @@
         <v>9</v>
       </c>
       <c r="G95" t="s">
-        <v>163</v>
+        <v>160</v>
       </c>
       <c r="H95" s="6" t="s">
-        <v>173</v>
+        <v>170</v>
       </c>
       <c r="I95" s="6" t="s">
-        <v>175</v>
+        <v>172</v>
       </c>
       <c r="J95">
         <f t="shared" si="3"/>
@@ -5131,7 +5131,7 @@
     </row>
     <row r="96" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A96" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
       <c r="B96" t="s">
         <v>3</v>
@@ -5149,13 +5149,13 @@
         <v>9</v>
       </c>
       <c r="G96" t="s">
-        <v>163</v>
+        <v>160</v>
       </c>
       <c r="H96" s="6" t="s">
-        <v>173</v>
+        <v>170</v>
       </c>
       <c r="I96" s="6" t="s">
-        <v>175</v>
+        <v>172</v>
       </c>
       <c r="J96">
         <f t="shared" si="3"/>
@@ -5172,10 +5172,10 @@
     </row>
     <row r="97" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A97" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
       <c r="B97" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C97">
         <v>4</v>
@@ -5190,13 +5190,13 @@
         <v>10</v>
       </c>
       <c r="G97" s="6" t="s">
-        <v>165</v>
+        <v>162</v>
       </c>
       <c r="H97" s="6" t="s">
-        <v>173</v>
+        <v>170</v>
       </c>
       <c r="I97" s="6" t="s">
-        <v>175</v>
+        <v>172</v>
       </c>
       <c r="J97">
         <f t="shared" si="3"/>
@@ -5213,7 +5213,7 @@
     </row>
     <row r="98" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A98" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
       <c r="B98" t="s">
         <v>3</v>
@@ -5231,10 +5231,10 @@
         <v>9</v>
       </c>
       <c r="G98" t="s">
-        <v>163</v>
+        <v>160</v>
       </c>
       <c r="H98" s="6" t="s">
-        <v>173</v>
+        <v>170</v>
       </c>
       <c r="J98">
         <f t="shared" si="3"/>
@@ -5251,7 +5251,7 @@
     </row>
     <row r="99" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A99" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
       <c r="B99" t="s">
         <v>3</v>
@@ -5269,13 +5269,13 @@
         <v>8</v>
       </c>
       <c r="G99" s="6" t="s">
-        <v>162</v>
+        <v>159</v>
       </c>
       <c r="H99" s="6" t="s">
-        <v>173</v>
+        <v>170</v>
       </c>
       <c r="I99" s="6" t="s">
-        <v>175</v>
+        <v>172</v>
       </c>
       <c r="J99">
         <f t="shared" si="3"/>
@@ -5292,10 +5292,10 @@
     </row>
     <row r="100" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A100" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
       <c r="B100" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C100">
         <v>3</v>
@@ -5310,7 +5310,7 @@
         <v>8</v>
       </c>
       <c r="H100" s="6" t="s">
-        <v>173</v>
+        <v>170</v>
       </c>
       <c r="J100">
         <f t="shared" si="3"/>
@@ -5327,7 +5327,7 @@
     </row>
     <row r="101" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A101" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
       <c r="B101" t="s">
         <v>7</v>
@@ -5345,10 +5345,10 @@
         <v>8</v>
       </c>
       <c r="G101" t="s">
-        <v>154</v>
+        <v>151</v>
       </c>
       <c r="H101" s="6" t="s">
-        <v>173</v>
+        <v>170</v>
       </c>
       <c r="J101">
         <f t="shared" si="3"/>
@@ -5365,7 +5365,7 @@
     </row>
     <row r="102" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A102" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
       <c r="B102" t="s">
         <v>7</v>
@@ -5383,10 +5383,10 @@
         <v>8</v>
       </c>
       <c r="G102" s="6" t="s">
-        <v>166</v>
+        <v>163</v>
       </c>
       <c r="H102" s="6" t="s">
-        <v>173</v>
+        <v>170</v>
       </c>
       <c r="J102">
         <f t="shared" si="3"/>
@@ -5403,7 +5403,7 @@
     </row>
     <row r="103" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A103" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
       <c r="B103" t="s">
         <v>10</v>
@@ -5421,10 +5421,10 @@
         <v>9</v>
       </c>
       <c r="G103" s="6" t="s">
-        <v>162</v>
+        <v>159</v>
       </c>
       <c r="H103" s="6" t="s">
-        <v>173</v>
+        <v>170</v>
       </c>
       <c r="J103">
         <f t="shared" si="3"/>
@@ -5441,7 +5441,7 @@
     </row>
     <row r="104" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A104" t="s">
-        <v>105</v>
+        <v>102</v>
       </c>
       <c r="B104" t="s">
         <v>7</v>
@@ -5459,10 +5459,10 @@
         <v>9</v>
       </c>
       <c r="G104" s="6" t="s">
-        <v>168</v>
+        <v>165</v>
       </c>
       <c r="H104" s="6" t="s">
-        <v>173</v>
+        <v>170</v>
       </c>
       <c r="J104">
         <f t="shared" si="3"/>
@@ -5479,7 +5479,7 @@
     </row>
     <row r="105" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A105" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
       <c r="B105" t="s">
         <v>3</v>
@@ -5497,10 +5497,10 @@
         <v>8</v>
       </c>
       <c r="G105" s="6" t="s">
-        <v>162</v>
+        <v>159</v>
       </c>
       <c r="H105" s="6" t="s">
-        <v>173</v>
+        <v>170</v>
       </c>
       <c r="J105">
         <f t="shared" si="3"/>
@@ -5517,7 +5517,7 @@
     </row>
     <row r="106" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A106" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
       <c r="B106" t="s">
         <v>3</v>
@@ -5535,10 +5535,10 @@
         <v>8</v>
       </c>
       <c r="G106" s="6" t="s">
-        <v>162</v>
+        <v>159</v>
       </c>
       <c r="H106" s="6" t="s">
-        <v>173</v>
+        <v>170</v>
       </c>
       <c r="J106">
         <f t="shared" si="3"/>
@@ -5555,7 +5555,7 @@
     </row>
     <row r="107" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A107" t="s">
-        <v>108</v>
+        <v>105</v>
       </c>
       <c r="B107" t="s">
         <v>5</v>
@@ -5573,10 +5573,10 @@
         <v>8</v>
       </c>
       <c r="H107" s="6" t="s">
+        <v>170</v>
+      </c>
+      <c r="I107" s="6" t="s">
         <v>173</v>
-      </c>
-      <c r="I107" s="6" t="s">
-        <v>176</v>
       </c>
       <c r="J107">
         <f t="shared" si="3"/>
@@ -5593,7 +5593,7 @@
     </row>
     <row r="108" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A108" t="s">
-        <v>109</v>
+        <v>106</v>
       </c>
       <c r="B108" t="s">
         <v>3</v>
@@ -5611,13 +5611,13 @@
         <v>8</v>
       </c>
       <c r="G108" s="6" t="s">
-        <v>165</v>
+        <v>162</v>
       </c>
       <c r="H108" s="6" t="s">
-        <v>173</v>
+        <v>170</v>
       </c>
       <c r="I108" s="6" t="s">
-        <v>175</v>
+        <v>172</v>
       </c>
       <c r="J108">
         <f t="shared" si="3"/>
@@ -5634,7 +5634,7 @@
     </row>
     <row r="109" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A109" t="s">
-        <v>110</v>
+        <v>107</v>
       </c>
       <c r="B109" t="s">
         <v>3</v>
@@ -5652,13 +5652,13 @@
         <v>8</v>
       </c>
       <c r="G109" s="6" t="s">
-        <v>165</v>
+        <v>162</v>
       </c>
       <c r="H109" s="6" t="s">
-        <v>173</v>
+        <v>170</v>
       </c>
       <c r="I109" s="6" t="s">
-        <v>175</v>
+        <v>172</v>
       </c>
       <c r="J109">
         <f t="shared" si="3"/>
@@ -5675,10 +5675,10 @@
     </row>
     <row r="110" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A110" t="s">
-        <v>111</v>
+        <v>108</v>
       </c>
       <c r="B110" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C110">
         <v>2</v>
@@ -5693,13 +5693,13 @@
         <v>7</v>
       </c>
       <c r="G110" s="6" t="s">
-        <v>162</v>
+        <v>159</v>
       </c>
       <c r="H110" s="6" t="s">
+        <v>170</v>
+      </c>
+      <c r="I110" s="6" t="s">
         <v>173</v>
-      </c>
-      <c r="I110" s="6" t="s">
-        <v>176</v>
       </c>
       <c r="J110">
         <f t="shared" si="3"/>
@@ -5716,7 +5716,7 @@
     </row>
     <row r="111" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A111" t="s">
-        <v>112</v>
+        <v>109</v>
       </c>
       <c r="B111" t="s">
         <v>3</v>
@@ -5734,10 +5734,10 @@
         <v>7</v>
       </c>
       <c r="H111" s="6" t="s">
-        <v>173</v>
+        <v>170</v>
       </c>
       <c r="I111" s="6" t="s">
-        <v>175</v>
+        <v>172</v>
       </c>
       <c r="J111">
         <f t="shared" si="3"/>
@@ -5754,7 +5754,7 @@
     </row>
     <row r="112" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A112" t="s">
-        <v>113</v>
+        <v>110</v>
       </c>
       <c r="B112" t="s">
         <v>3</v>
@@ -5772,13 +5772,13 @@
         <v>8</v>
       </c>
       <c r="G112" t="s">
-        <v>158</v>
+        <v>155</v>
       </c>
       <c r="H112" s="6" t="s">
-        <v>173</v>
+        <v>170</v>
       </c>
       <c r="I112" s="6" t="s">
-        <v>175</v>
+        <v>172</v>
       </c>
       <c r="J112">
         <f t="shared" si="3"/>
@@ -5795,7 +5795,7 @@
     </row>
     <row r="113" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A113" t="s">
-        <v>114</v>
+        <v>111</v>
       </c>
       <c r="B113" t="s">
         <v>3</v>
@@ -5813,13 +5813,13 @@
         <v>8</v>
       </c>
       <c r="G113" s="6" t="s">
-        <v>165</v>
+        <v>162</v>
       </c>
       <c r="H113" s="6" t="s">
-        <v>173</v>
+        <v>170</v>
       </c>
       <c r="I113" s="6" t="s">
-        <v>175</v>
+        <v>172</v>
       </c>
       <c r="J113">
         <f t="shared" si="3"/>
@@ -5836,7 +5836,7 @@
     </row>
     <row r="114" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A114" t="s">
-        <v>115</v>
+        <v>112</v>
       </c>
       <c r="B114" t="s">
         <v>3</v>
@@ -5854,10 +5854,10 @@
         <v>8</v>
       </c>
       <c r="G114" s="6" t="s">
-        <v>162</v>
+        <v>159</v>
       </c>
       <c r="H114" s="6" t="s">
-        <v>173</v>
+        <v>170</v>
       </c>
       <c r="J114">
         <f t="shared" si="3"/>
@@ -5874,7 +5874,7 @@
     </row>
     <row r="115" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A115" t="s">
-        <v>116</v>
+        <v>113</v>
       </c>
       <c r="B115" t="s">
         <v>3</v>
@@ -5892,7 +5892,7 @@
         <v>9</v>
       </c>
       <c r="H115" s="6" t="s">
-        <v>173</v>
+        <v>170</v>
       </c>
       <c r="J115">
         <f t="shared" si="3"/>
@@ -5909,7 +5909,7 @@
     </row>
     <row r="116" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A116" t="s">
-        <v>159</v>
+        <v>156</v>
       </c>
       <c r="B116" t="s">
         <v>7</v>
@@ -5927,10 +5927,10 @@
         <v>9</v>
       </c>
       <c r="H116" s="6" t="s">
-        <v>173</v>
+        <v>170</v>
       </c>
       <c r="I116" s="6" t="s">
-        <v>175</v>
+        <v>172</v>
       </c>
       <c r="J116">
         <f t="shared" si="3"/>
@@ -5947,7 +5947,7 @@
     </row>
     <row r="117" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A117" t="s">
-        <v>117</v>
+        <v>114</v>
       </c>
       <c r="B117" t="s">
         <v>7</v>
@@ -5965,7 +5965,7 @@
         <v>8</v>
       </c>
       <c r="H117" s="6" t="s">
-        <v>173</v>
+        <v>170</v>
       </c>
       <c r="J117">
         <f t="shared" si="3"/>
@@ -5982,7 +5982,7 @@
     </row>
     <row r="118" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A118" t="s">
-        <v>118</v>
+        <v>115</v>
       </c>
       <c r="B118" t="s">
         <v>10</v>
@@ -6000,10 +6000,10 @@
         <v>8</v>
       </c>
       <c r="H118" s="6" t="s">
+        <v>170</v>
+      </c>
+      <c r="I118" s="6" t="s">
         <v>173</v>
-      </c>
-      <c r="I118" s="6" t="s">
-        <v>176</v>
       </c>
       <c r="J118">
         <f t="shared" si="3"/>
@@ -6020,7 +6020,7 @@
     </row>
     <row r="119" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A119" t="s">
-        <v>119</v>
+        <v>116</v>
       </c>
       <c r="B119" t="s">
         <v>3</v>
@@ -6038,13 +6038,13 @@
         <v>8</v>
       </c>
       <c r="G119" s="6" t="s">
-        <v>162</v>
+        <v>159</v>
       </c>
       <c r="H119" s="6" t="s">
-        <v>173</v>
+        <v>170</v>
       </c>
       <c r="I119" s="6" t="s">
-        <v>175</v>
+        <v>172</v>
       </c>
       <c r="J119">
         <f t="shared" si="3"/>
@@ -6061,10 +6061,10 @@
     </row>
     <row r="120" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A120" t="s">
-        <v>120</v>
+        <v>117</v>
       </c>
       <c r="B120" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C120">
         <v>3</v>
@@ -6079,10 +6079,10 @@
         <v>7</v>
       </c>
       <c r="G120" s="6" t="s">
-        <v>162</v>
+        <v>159</v>
       </c>
       <c r="H120" s="6" t="s">
-        <v>173</v>
+        <v>170</v>
       </c>
       <c r="J120">
         <f t="shared" si="3"/>
@@ -6099,10 +6099,10 @@
     </row>
     <row r="121" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A121" t="s">
-        <v>121</v>
+        <v>118</v>
       </c>
       <c r="B121" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C121">
         <v>3</v>
@@ -6117,10 +6117,10 @@
         <v>8</v>
       </c>
       <c r="G121" s="6" t="s">
-        <v>162</v>
+        <v>159</v>
       </c>
       <c r="H121" s="6" t="s">
-        <v>173</v>
+        <v>170</v>
       </c>
       <c r="J121">
         <f t="shared" si="3"/>
@@ -6137,7 +6137,7 @@
     </row>
     <row r="122" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A122" t="s">
-        <v>122</v>
+        <v>119</v>
       </c>
       <c r="B122" t="s">
         <v>3</v>
@@ -6155,10 +6155,10 @@
         <v>8</v>
       </c>
       <c r="G122" s="6" t="s">
-        <v>162</v>
+        <v>159</v>
       </c>
       <c r="H122" s="6" t="s">
-        <v>173</v>
+        <v>170</v>
       </c>
       <c r="J122">
         <f t="shared" si="3"/>
@@ -6175,10 +6175,10 @@
     </row>
     <row r="123" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A123" t="s">
-        <v>123</v>
+        <v>120</v>
       </c>
       <c r="B123" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C123">
         <v>3</v>
@@ -6193,13 +6193,13 @@
         <v>9</v>
       </c>
       <c r="G123" s="6" t="s">
-        <v>162</v>
+        <v>159</v>
       </c>
       <c r="H123" s="6" t="s">
-        <v>173</v>
+        <v>170</v>
       </c>
       <c r="I123" s="6" t="s">
-        <v>175</v>
+        <v>172</v>
       </c>
       <c r="J123">
         <f t="shared" si="3"/>
@@ -6216,10 +6216,10 @@
     </row>
     <row r="124" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A124" t="s">
-        <v>124</v>
+        <v>121</v>
       </c>
       <c r="B124" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C124">
         <v>3</v>
@@ -6234,10 +6234,10 @@
         <v>9</v>
       </c>
       <c r="G124" s="6" t="s">
-        <v>162</v>
+        <v>159</v>
       </c>
       <c r="H124" s="6" t="s">
-        <v>173</v>
+        <v>170</v>
       </c>
       <c r="J124">
         <f t="shared" si="3"/>
@@ -6254,7 +6254,7 @@
     </row>
     <row r="125" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A125" t="s">
-        <v>125</v>
+        <v>122</v>
       </c>
       <c r="B125" t="s">
         <v>3</v>
@@ -6272,13 +6272,13 @@
         <v>9</v>
       </c>
       <c r="G125" t="s">
-        <v>154</v>
+        <v>151</v>
       </c>
       <c r="H125" s="6" t="s">
-        <v>173</v>
+        <v>170</v>
       </c>
       <c r="I125" s="6" t="s">
-        <v>175</v>
+        <v>172</v>
       </c>
       <c r="J125">
         <f t="shared" si="3"/>
@@ -6295,7 +6295,7 @@
     </row>
     <row r="126" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A126" t="s">
-        <v>126</v>
+        <v>123</v>
       </c>
       <c r="B126" t="s">
         <v>3</v>
@@ -6313,7 +6313,7 @@
         <v>8</v>
       </c>
       <c r="H126" s="6" t="s">
-        <v>173</v>
+        <v>170</v>
       </c>
       <c r="J126">
         <f t="shared" si="3"/>
@@ -6330,7 +6330,7 @@
     </row>
     <row r="127" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A127" t="s">
-        <v>127</v>
+        <v>124</v>
       </c>
       <c r="B127" t="s">
         <v>5</v>
@@ -6348,13 +6348,13 @@
         <v>9</v>
       </c>
       <c r="G127" s="6" t="s">
-        <v>167</v>
+        <v>164</v>
       </c>
       <c r="H127" s="6" t="s">
-        <v>173</v>
+        <v>170</v>
       </c>
       <c r="I127" s="6" t="s">
-        <v>175</v>
+        <v>172</v>
       </c>
       <c r="J127">
         <f t="shared" si="3"/>
@@ -6371,7 +6371,7 @@
     </row>
     <row r="128" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A128" t="s">
-        <v>128</v>
+        <v>125</v>
       </c>
       <c r="B128" t="s">
         <v>3</v>
@@ -6389,13 +6389,13 @@
         <v>9</v>
       </c>
       <c r="G128" s="6" t="s">
-        <v>162</v>
+        <v>159</v>
       </c>
       <c r="H128" s="6" t="s">
-        <v>173</v>
+        <v>170</v>
       </c>
       <c r="I128" s="6" t="s">
-        <v>175</v>
+        <v>172</v>
       </c>
       <c r="J128">
         <f t="shared" si="3"/>
@@ -6412,7 +6412,7 @@
     </row>
     <row r="129" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A129" t="s">
-        <v>129</v>
+        <v>126</v>
       </c>
       <c r="B129" t="s">
         <v>3</v>
@@ -6430,10 +6430,10 @@
         <v>8</v>
       </c>
       <c r="G129" s="6" t="s">
-        <v>162</v>
+        <v>159</v>
       </c>
       <c r="H129" s="6" t="s">
-        <v>173</v>
+        <v>170</v>
       </c>
       <c r="J129">
         <f t="shared" ref="J129:J142" si="6">D129-C129</f>
@@ -6450,7 +6450,7 @@
     </row>
     <row r="130" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A130" t="s">
-        <v>130</v>
+        <v>127</v>
       </c>
       <c r="B130" t="s">
         <v>3</v>
@@ -6468,13 +6468,13 @@
         <v>8</v>
       </c>
       <c r="G130" s="6" t="s">
-        <v>162</v>
+        <v>159</v>
       </c>
       <c r="H130" s="6" t="s">
-        <v>173</v>
+        <v>170</v>
       </c>
       <c r="I130" s="6" t="s">
-        <v>175</v>
+        <v>172</v>
       </c>
       <c r="J130">
         <f t="shared" si="6"/>
@@ -6491,10 +6491,10 @@
     </row>
     <row r="131" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A131" t="s">
-        <v>131</v>
+        <v>128</v>
       </c>
       <c r="B131" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C131">
         <v>3</v>
@@ -6509,10 +6509,10 @@
         <v>8</v>
       </c>
       <c r="H131" s="6" t="s">
-        <v>173</v>
+        <v>170</v>
       </c>
       <c r="I131" s="6" t="s">
-        <v>175</v>
+        <v>172</v>
       </c>
       <c r="J131">
         <f t="shared" si="6"/>
@@ -6529,10 +6529,10 @@
     </row>
     <row r="132" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A132" t="s">
-        <v>132</v>
+        <v>129</v>
       </c>
       <c r="B132" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C132">
         <v>4</v>
@@ -6547,13 +6547,13 @@
         <v>9</v>
       </c>
       <c r="G132" s="6" t="s">
-        <v>162</v>
+        <v>159</v>
       </c>
       <c r="H132" s="6" t="s">
-        <v>173</v>
+        <v>170</v>
       </c>
       <c r="I132" s="6" t="s">
-        <v>175</v>
+        <v>172</v>
       </c>
       <c r="J132">
         <f t="shared" si="6"/>
@@ -6570,7 +6570,7 @@
     </row>
     <row r="133" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A133" t="s">
-        <v>133</v>
+        <v>130</v>
       </c>
       <c r="B133" t="s">
         <v>3</v>
@@ -6588,10 +6588,10 @@
         <v>8</v>
       </c>
       <c r="G133" s="6" t="s">
-        <v>162</v>
+        <v>159</v>
       </c>
       <c r="H133" s="6" t="s">
-        <v>173</v>
+        <v>170</v>
       </c>
       <c r="J133">
         <f t="shared" si="6"/>
@@ -6608,10 +6608,10 @@
     </row>
     <row r="134" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A134" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="B134" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C134">
         <v>4</v>
@@ -6626,10 +6626,10 @@
         <v>8</v>
       </c>
       <c r="G134" s="6" t="s">
-        <v>162</v>
+        <v>159</v>
       </c>
       <c r="H134" s="6" t="s">
-        <v>173</v>
+        <v>170</v>
       </c>
       <c r="J134">
         <f t="shared" si="6"/>
@@ -6646,7 +6646,7 @@
     </row>
     <row r="135" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A135" t="s">
-        <v>135</v>
+        <v>132</v>
       </c>
       <c r="B135" t="s">
         <v>5</v>
@@ -6664,10 +6664,10 @@
         <v>8</v>
       </c>
       <c r="G135" s="6" t="s">
-        <v>168</v>
+        <v>165</v>
       </c>
       <c r="H135" s="6" t="s">
-        <v>173</v>
+        <v>170</v>
       </c>
       <c r="J135">
         <f t="shared" si="6"/>
@@ -6684,7 +6684,7 @@
     </row>
     <row r="136" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A136" t="s">
-        <v>136</v>
+        <v>133</v>
       </c>
       <c r="B136" t="s">
         <v>3</v>
@@ -6702,13 +6702,13 @@
         <v>9</v>
       </c>
       <c r="G136" s="6" t="s">
-        <v>162</v>
+        <v>159</v>
       </c>
       <c r="H136" s="6" t="s">
-        <v>173</v>
+        <v>170</v>
       </c>
       <c r="I136" s="6" t="s">
-        <v>175</v>
+        <v>172</v>
       </c>
       <c r="J136">
         <f t="shared" si="6"/>
@@ -6725,7 +6725,7 @@
     </row>
     <row r="137" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A137" t="s">
-        <v>137</v>
+        <v>134</v>
       </c>
       <c r="B137" t="s">
         <v>3</v>
@@ -6743,10 +6743,10 @@
         <v>8</v>
       </c>
       <c r="G137" s="6" t="s">
-        <v>162</v>
+        <v>159</v>
       </c>
       <c r="H137" s="6" t="s">
-        <v>173</v>
+        <v>170</v>
       </c>
       <c r="J137">
         <f t="shared" si="6"/>
@@ -6763,7 +6763,7 @@
     </row>
     <row r="138" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A138" t="s">
-        <v>138</v>
+        <v>135</v>
       </c>
       <c r="B138" t="s">
         <v>3</v>
@@ -6781,13 +6781,13 @@
         <v>8</v>
       </c>
       <c r="G138" s="6" t="s">
-        <v>162</v>
+        <v>159</v>
       </c>
       <c r="H138" s="6" t="s">
-        <v>173</v>
+        <v>170</v>
       </c>
       <c r="I138" s="6" t="s">
-        <v>175</v>
+        <v>172</v>
       </c>
       <c r="J138">
         <f t="shared" si="6"/>
@@ -6804,7 +6804,7 @@
     </row>
     <row r="139" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A139" t="s">
-        <v>139</v>
+        <v>136</v>
       </c>
       <c r="B139" t="s">
         <v>5</v>
@@ -6822,10 +6822,10 @@
         <v>8</v>
       </c>
       <c r="G139" s="6" t="s">
-        <v>168</v>
+        <v>165</v>
       </c>
       <c r="H139" s="6" t="s">
-        <v>173</v>
+        <v>170</v>
       </c>
       <c r="J139">
         <f t="shared" si="6"/>
@@ -6842,10 +6842,10 @@
     </row>
     <row r="140" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A140" t="s">
-        <v>140</v>
+        <v>137</v>
       </c>
       <c r="B140" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="C140">
         <v>3</v>
@@ -6874,7 +6874,7 @@
     </row>
     <row r="141" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A141" t="s">
-        <v>141</v>
+        <v>138</v>
       </c>
       <c r="B141" t="s">
         <v>3</v>
@@ -6892,13 +6892,13 @@
         <v>8</v>
       </c>
       <c r="G141" t="s">
-        <v>160</v>
+        <v>157</v>
       </c>
       <c r="H141" s="6" t="s">
-        <v>173</v>
+        <v>170</v>
       </c>
       <c r="I141" s="6" t="s">
-        <v>177</v>
+        <v>174</v>
       </c>
       <c r="J141">
         <f t="shared" si="6"/>
@@ -6915,7 +6915,7 @@
     </row>
     <row r="142" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A142" t="s">
-        <v>142</v>
+        <v>139</v>
       </c>
       <c r="B142" t="s">
         <v>3</v>
@@ -6933,10 +6933,10 @@
         <v>7</v>
       </c>
       <c r="G142" s="6" t="s">
-        <v>162</v>
+        <v>159</v>
       </c>
       <c r="H142" s="6" t="s">
-        <v>173</v>
+        <v>170</v>
       </c>
       <c r="J142">
         <f t="shared" si="6"/>
@@ -6970,7 +6970,7 @@
   <dimension ref="A1:B13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B14" sqref="B14"/>
+      <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -6981,10 +6981,10 @@
   <sheetData>
     <row r="1" spans="1:2" ht="17" x14ac:dyDescent="0.2">
       <c r="A1" s="4" t="s">
-        <v>144</v>
+        <v>141</v>
       </c>
       <c r="B1" s="5" t="s">
-        <v>143</v>
+        <v>140</v>
       </c>
     </row>
     <row r="2" spans="1:2" ht="17" x14ac:dyDescent="0.2">
@@ -6992,7 +6992,7 @@
         <v>0</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>151</v>
+        <v>148</v>
       </c>
     </row>
     <row r="3" spans="1:2" ht="17" x14ac:dyDescent="0.2">
@@ -7000,87 +7000,87 @@
         <v>1</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>152</v>
+        <v>149</v>
       </c>
     </row>
     <row r="4" spans="1:2" ht="51" x14ac:dyDescent="0.2">
       <c r="A4" s="3" t="s">
-        <v>147</v>
+        <v>144</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>161</v>
+        <v>158</v>
       </c>
     </row>
     <row r="5" spans="1:2" ht="17" x14ac:dyDescent="0.2">
       <c r="A5" s="3" t="s">
-        <v>148</v>
+        <v>145</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>187</v>
+        <v>184</v>
       </c>
     </row>
     <row r="6" spans="1:2" ht="102" x14ac:dyDescent="0.2">
       <c r="A6" s="4" t="s">
-        <v>149</v>
+        <v>146</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>188</v>
+        <v>185</v>
       </c>
     </row>
     <row r="7" spans="1:2" ht="85" x14ac:dyDescent="0.2">
       <c r="A7" s="4" t="s">
-        <v>150</v>
+        <v>147</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>189</v>
+        <v>186</v>
       </c>
     </row>
     <row r="8" spans="1:2" ht="17" x14ac:dyDescent="0.2">
       <c r="A8" s="4" t="s">
-        <v>170</v>
+        <v>167</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>190</v>
+        <v>187</v>
       </c>
     </row>
     <row r="9" spans="1:2" ht="34" x14ac:dyDescent="0.2">
       <c r="A9" s="4" t="s">
-        <v>171</v>
+        <v>168</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>191</v>
+        <v>188</v>
       </c>
     </row>
     <row r="10" spans="1:2" ht="34" x14ac:dyDescent="0.2">
       <c r="A10" s="4" t="s">
-        <v>174</v>
+        <v>171</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>192</v>
+        <v>189</v>
       </c>
     </row>
     <row r="11" spans="1:2" ht="17" x14ac:dyDescent="0.2">
       <c r="A11" s="4" t="s">
-        <v>184</v>
+        <v>181</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>193</v>
+        <v>190</v>
       </c>
     </row>
     <row r="12" spans="1:2" ht="17" x14ac:dyDescent="0.2">
       <c r="A12" s="4" t="s">
-        <v>185</v>
+        <v>182</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>194</v>
+        <v>191</v>
       </c>
     </row>
     <row r="13" spans="1:2" ht="17" x14ac:dyDescent="0.2">
       <c r="A13" s="4" t="s">
-        <v>186</v>
+        <v>183</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>195</v>
+        <v>192</v>
       </c>
     </row>
   </sheetData>

</xml_diff>